<commit_message>
Minor edit to ECO
</commit_message>
<xml_diff>
--- a/COMCRD.ECO.xlsx
+++ b/COMCRD.ECO.xlsx
@@ -59,7 +59,7 @@
     <t>Ethan Dale</t>
   </si>
   <si>
-    <t>Initial production run of COMMANDCARD.</t>
+    <t>Initial production run of COMCRD v1.0.</t>
   </si>
 </sst>
 </file>
@@ -208,20 +208,20 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.7888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.262962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="13.8962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.7407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.7703703703704"/>
-    <col collapsed="false" hidden="false" max="1022" min="11" style="1" width="20.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="20.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.0259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.5074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.0814814814815"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="15.0185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.5925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1022" min="11" style="1" width="22.5259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="22.5259259259259"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -324,7 +324,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1.16666666666667" bottom="1" header="1" footer="0.5"/>
-  <pageSetup paperSize="1" scale="55" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;"Times New Roman,Regular"COMCRD.ECO</oddHeader>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>

</xml_diff>